<commit_message>
database: deposit, withdraw, record (Transferhistorie) sind erstellt
</commit_message>
<xml_diff>
--- a/transferhistorie.xlsx
+++ b/transferhistorie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonnt\Documents\GitHub\verein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC16FD1A-01C5-40ED-A0A5-BA98F40B5D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B40B05-254D-48B8-B6DF-482CC757D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01D25E55-572D-42EC-8F96-3008A9472777}"/>
   </bookViews>
@@ -36,23 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>department</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>operation</t>
   </si>
   <si>
     <t>tanzen</t>
   </si>
   <si>
-    <t>01.01.2021</t>
-  </si>
-  <si>
     <t>fussbal</t>
   </si>
   <si>
@@ -69,6 +63,9 @@
   </si>
   <si>
     <t>+2</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -444,41 +441,40 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -488,31 +484,31 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>-2</v>

</xml_diff>